<commit_message>
KIBON-288: Individuellen Zuschlag zum Erwerbspensum entfernen: Statistiken angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\G$\hefr\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD09EE2D-0E2C-49B3-B2E5-B90A077DEF69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="360" windowWidth="16380" windowHeight="8190" tabRatio="606"/>
+    <workbookView xWindow="975" yWindow="360" windowWidth="16380" windowHeight="8190" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>Parameter</t>
   </si>
@@ -122,9 +128,6 @@
     <t>RAV</t>
   </si>
   <si>
-    <t>Zuschlag</t>
-  </si>
-  <si>
     <t>{institution}</t>
   </si>
   <si>
@@ -182,9 +185,6 @@
     <t>{gs1EwpRav}</t>
   </si>
   <si>
-    <t>{gs1EwpZuschlag}</t>
-  </si>
-  <si>
     <t>{gs1EwpGesundhtl}</t>
   </si>
   <si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>{gs2EwpRav}</t>
-  </si>
-  <si>
-    <t>{gs2EwpZuschlag}</t>
   </si>
   <si>
     <t>{gs2EwpGesundhtl}</t>
@@ -293,7 +290,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
@@ -482,40 +479,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,7 +600,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -678,6 +675,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -713,6 +727,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -888,14 +919,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AX9"/>
+  <dimension ref="A1:AV9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ1" sqref="AJ1:AJ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,26 +935,26 @@
     <col min="3" max="3" width="15.7109375" style="1"/>
     <col min="4" max="5" width="17"/>
     <col min="7" max="15" width="8.7109375"/>
-    <col min="16" max="21" width="10.7109375"/>
-    <col min="22" max="22" width="24.140625"/>
-    <col min="23" max="31" width="8.7109375"/>
-    <col min="32" max="37" width="10.7109375"/>
-    <col min="38" max="38" width="24.140625"/>
-    <col min="39" max="39" width="9.140625" customWidth="1"/>
-    <col min="41" max="41" width="6.5703125"/>
-    <col min="42" max="42" width="18.140625"/>
-    <col min="44" max="44" width="23.28515625"/>
-    <col min="45" max="45" width="9.28515625"/>
-    <col min="46" max="46" width="25.42578125"/>
-    <col min="47" max="47" width="27.5703125"/>
-    <col min="48" max="48" width="10.5703125"/>
-    <col min="49" max="49" width="21.140625" customWidth="1"/>
-    <col min="50" max="1003" width="10.5703125"/>
+    <col min="16" max="20" width="10.7109375"/>
+    <col min="21" max="21" width="24.140625"/>
+    <col min="22" max="30" width="8.7109375"/>
+    <col min="31" max="35" width="10.7109375"/>
+    <col min="36" max="36" width="24.140625"/>
+    <col min="37" max="37" width="9.140625" customWidth="1"/>
+    <col min="39" max="39" width="6.5703125"/>
+    <col min="40" max="40" width="18.140625"/>
+    <col min="42" max="42" width="23.28515625"/>
+    <col min="43" max="43" width="9.28515625"/>
+    <col min="44" max="44" width="25.42578125"/>
+    <col min="45" max="45" width="27.5703125"/>
+    <col min="46" max="46" width="10.5703125"/>
+    <col min="47" max="47" width="21.140625" customWidth="1"/>
+    <col min="48" max="1001" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -931,10 +962,10 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -944,211 +975,207 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="6" spans="1:50" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="23" t="s">
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
-      <c r="AI6" s="24"/>
-      <c r="AJ6" s="24"/>
-      <c r="AK6" s="24"/>
-      <c r="AL6" s="24"/>
-      <c r="AM6" s="25" t="s">
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="21"/>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="30"/>
+      <c r="AG6" s="30"/>
+      <c r="AH6" s="30"/>
+      <c r="AI6" s="30"/>
+      <c r="AJ6" s="30"/>
+      <c r="AK6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="AN6" s="25"/>
-      <c r="AO6" s="25"/>
-      <c r="AP6" s="25" t="s">
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="AQ6" s="25"/>
-      <c r="AR6" s="25"/>
-      <c r="AS6" s="25"/>
-      <c r="AT6" s="25"/>
-      <c r="AU6" s="25" t="s">
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="23"/>
+      <c r="AQ6" s="23"/>
+      <c r="AR6" s="23"/>
+      <c r="AS6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="AV6" s="23" t="s">
+      <c r="AT6" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="23" t="s">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="23" t="s">
+      <c r="N7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="O7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="28" t="s">
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="X7" s="23" t="s">
+      <c r="W7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="Y7" s="23" t="s">
+      <c r="X7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Z7" s="23" t="s">
+      <c r="Y7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AA7" s="23" t="s">
+      <c r="Z7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AB7" s="23" t="s">
+      <c r="AA7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AC7" s="23" t="s">
+      <c r="AB7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="23" t="s">
+      <c r="AC7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="AE7" s="26" t="s">
+      <c r="AD7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AF7" s="26" t="s">
+      <c r="AE7" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AG7" s="27"/>
-      <c r="AH7" s="27"/>
-      <c r="AI7" s="27"/>
-      <c r="AJ7" s="27"/>
-      <c r="AK7" s="27"/>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="29" t="s">
+      <c r="AF7" s="25"/>
+      <c r="AG7" s="25"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="25"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AN7" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO7" s="25" t="s">
+      <c r="AL7" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="AP7" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ7" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="AR7" s="25" t="s">
+      <c r="AN7" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO7" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="AS7" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="AT7" s="25" t="s">
+      <c r="AQ7" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR7" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="AU7" s="25"/>
-      <c r="AV7" s="23"/>
+      <c r="AS7" s="23"/>
+      <c r="AT7" s="21"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
       <c r="P8" s="12" t="s">
         <v>4</v>
       </c>
@@ -1164,230 +1191,204 @@
       <c r="T8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="U8" s="12" t="s">
+      <c r="U8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK8" s="23"/>
+      <c r="AL8" s="28"/>
+      <c r="AM8" s="23"/>
+      <c r="AN8" s="28"/>
+      <c r="AO8" s="28"/>
+      <c r="AP8" s="23"/>
+      <c r="AQ8" s="23"/>
+      <c r="AR8" s="23"/>
+      <c r="AS8" s="23"/>
+      <c r="AT8" s="21"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="V8" s="13" t="s">
+      <c r="B9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" s="18" t="e">
+        <f>Q9+R9+S9+T9+#REF!+U9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="U9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W9" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL8" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM8" s="25"/>
-      <c r="AN8" s="32"/>
-      <c r="AO8" s="25"/>
-      <c r="AP8" s="32"/>
-      <c r="AQ8" s="32"/>
-      <c r="AR8" s="25"/>
-      <c r="AS8" s="25"/>
-      <c r="AT8" s="25"/>
-      <c r="AU8" s="25"/>
-      <c r="AV8" s="23"/>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" s="18" t="e">
-        <f>Q9+R9+S9+T9+U9+V9</f>
+      <c r="X9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE9" s="19" t="e">
+        <f>IF((AF9+AG9+AH9+AI9+#REF!+AJ9)&gt;0,AF9+AG9+AH9+AI9+#REF!+AJ9,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="T9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="U9" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="V9" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="W9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z9" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA9" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB9" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC9" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD9" s="11" t="s">
+      <c r="AF9" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="AE9" s="11" t="s">
+      <c r="AG9" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="AF9" s="19" t="e">
-        <f>IF((AG9+AH9+AI9+AJ9+AK9+AL9)&gt;0,AG9+AH9+AI9+AJ9+AK9+AL9,)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AG9" s="16" t="s">
+      <c r="AH9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="AH9" s="16" t="s">
+      <c r="AI9" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AI9" s="16" t="s">
+      <c r="AJ9" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="AJ9" s="16" t="s">
+      <c r="AK9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="AK9" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL9" s="16" t="s">
+      <c r="AL9" s="11" t="s">
         <v>69</v>
       </c>
       <c r="AM9" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="AN9" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO9" s="11" t="s">
-        <v>73</v>
+      <c r="AN9" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO9" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="AP9" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="AQ9" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="AR9" s="17" t="s">
-        <v>84</v>
+      <c r="AQ9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR9" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="AS9" s="11" t="s">
         <v>74</v>
       </c>
       <c r="AT9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AU9" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AV9" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AW9" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX9" s="8"/>
+      <c r="AV9" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AM7:AM8"/>
-    <mergeCell ref="AP6:AT6"/>
-    <mergeCell ref="AU6:AU8"/>
-    <mergeCell ref="AV6:AV8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AE8"/>
-    <mergeCell ref="AF7:AK7"/>
-    <mergeCell ref="AO7:AO8"/>
-    <mergeCell ref="AR7:AR8"/>
-    <mergeCell ref="AS7:AS8"/>
-    <mergeCell ref="AT7:AT8"/>
-    <mergeCell ref="AN7:AN8"/>
-    <mergeCell ref="AP7:AP8"/>
-    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:V6"/>
-    <mergeCell ref="W6:AL6"/>
-    <mergeCell ref="AM6:AO6"/>
+    <mergeCell ref="G6:U6"/>
+    <mergeCell ref="V6:AJ6"/>
+    <mergeCell ref="AK6:AM6"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
@@ -1397,14 +1398,28 @@
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="P7:T7"/>
+    <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS6:AS8"/>
+    <mergeCell ref="AT6:AT8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AI7"/>
+    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="AP7:AP8"/>
+    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="AR7:AR8"/>
+    <mergeCell ref="AL7:AL8"/>
+    <mergeCell ref="AN7:AN8"/>
+    <mergeCell ref="AO7:AO8"/>
     <mergeCell ref="X7:X8"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AK7:AK8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
directToDev: Excel Vorlage für Statistiken korrigiert
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\G$\hefr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD09EE2D-0E2C-49B3-B2E5-B90A077DEF69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E68D0E-D056-41F7-AEFC-C48A18CB4FF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="975" yWindow="360" windowWidth="16380" windowHeight="8190" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,40 +479,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,8 +925,8 @@
   </sheetPr>
   <dimension ref="A1:AV9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ1" sqref="AJ1:AJ1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,197 +985,197 @@
       <c r="C4"/>
     </row>
     <row r="6" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="21" t="s">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
-      <c r="AE6" s="30"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
-      <c r="AH6" s="30"/>
-      <c r="AI6" s="30"/>
-      <c r="AJ6" s="30"/>
-      <c r="AK6" s="23" t="s">
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="24"/>
+      <c r="AI6" s="24"/>
+      <c r="AJ6" s="24"/>
+      <c r="AK6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="23"/>
-      <c r="AN6" s="23" t="s">
+      <c r="AL6" s="25"/>
+      <c r="AM6" s="25"/>
+      <c r="AN6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="AO6" s="23"/>
-      <c r="AP6" s="23"/>
-      <c r="AQ6" s="23"/>
-      <c r="AR6" s="23"/>
-      <c r="AS6" s="23" t="s">
+      <c r="AO6" s="25"/>
+      <c r="AP6" s="25"/>
+      <c r="AQ6" s="25"/>
+      <c r="AR6" s="25"/>
+      <c r="AS6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="AT6" s="21" t="s">
+      <c r="AT6" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="21" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
       <c r="U7" s="9"/>
-      <c r="V7" s="31" t="s">
+      <c r="V7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="W7" s="21" t="s">
+      <c r="W7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="X7" s="21" t="s">
+      <c r="X7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="Y7" s="21" t="s">
+      <c r="Y7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="Z7" s="21" t="s">
+      <c r="Z7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="AA7" s="21" t="s">
+      <c r="AA7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="21" t="s">
+      <c r="AB7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AC7" s="21" t="s">
+      <c r="AC7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AD7" s="24" t="s">
+      <c r="AD7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="AE7" s="24" t="s">
+      <c r="AE7" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="AF7" s="25"/>
-      <c r="AG7" s="25"/>
-      <c r="AH7" s="25"/>
-      <c r="AI7" s="25"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="27"/>
+      <c r="AI7" s="27"/>
       <c r="AJ7" s="9"/>
-      <c r="AK7" s="22" t="s">
+      <c r="AK7" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AL7" s="27" t="s">
+      <c r="AL7" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="AM7" s="23" t="s">
+      <c r="AM7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="AN7" s="27" t="s">
+      <c r="AN7" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="AO7" s="27" t="s">
+      <c r="AO7" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="AP7" s="23" t="s">
+      <c r="AP7" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="AQ7" s="26" t="s">
+      <c r="AQ7" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="AR7" s="23" t="s">
+      <c r="AR7" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="AS7" s="23"/>
-      <c r="AT7" s="21"/>
+      <c r="AS7" s="25"/>
+      <c r="AT7" s="23"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
       <c r="P8" s="12" t="s">
         <v>4</v>
       </c>
@@ -1194,15 +1194,15 @@
       <c r="U8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23"/>
       <c r="AE8" s="12" t="s">
         <v>4</v>
       </c>
@@ -1221,16 +1221,16 @@
       <c r="AJ8" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="AK8" s="23"/>
-      <c r="AL8" s="28"/>
-      <c r="AM8" s="23"/>
-      <c r="AN8" s="28"/>
-      <c r="AO8" s="28"/>
-      <c r="AP8" s="23"/>
-      <c r="AQ8" s="23"/>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="23"/>
-      <c r="AT8" s="21"/>
+      <c r="AK8" s="25"/>
+      <c r="AL8" s="31"/>
+      <c r="AM8" s="25"/>
+      <c r="AN8" s="31"/>
+      <c r="AO8" s="31"/>
+      <c r="AP8" s="25"/>
+      <c r="AQ8" s="25"/>
+      <c r="AR8" s="25"/>
+      <c r="AS8" s="25"/>
+      <c r="AT8" s="23"/>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -1279,7 +1279,7 @@
         <v>46</v>
       </c>
       <c r="P9" s="18" t="e">
-        <f>Q9+R9+S9+T9+#REF!+U9</f>
+        <f>Q9+R9+S9+T9+U9</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q9" s="16" t="s">
@@ -1325,7 +1325,7 @@
         <v>61</v>
       </c>
       <c r="AE9" s="19" t="e">
-        <f>IF((AF9+AG9+AH9+AI9+#REF!+AJ9)&gt;0,AF9+AG9+AH9+AI9+#REF!+AJ9,)</f>
+        <f>IF((AF9+AG9+AH9+AI9+AJ9)&gt;0,AF9+AG9+AH9+AI9+AJ9,)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AF9" s="16" t="s">
@@ -1380,11 +1380,25 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AK7:AK8"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS6:AS8"/>
+    <mergeCell ref="AT6:AT8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AI7"/>
+    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="AP7:AP8"/>
+    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="AR7:AR8"/>
+    <mergeCell ref="AL7:AL8"/>
+    <mergeCell ref="AN7:AN8"/>
+    <mergeCell ref="AO7:AO8"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="G6:U6"/>
     <mergeCell ref="V6:AJ6"/>
@@ -1401,25 +1415,11 @@
     <mergeCell ref="P7:T7"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS6:AS8"/>
-    <mergeCell ref="AT6:AT8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AI7"/>
-    <mergeCell ref="AM7:AM8"/>
-    <mergeCell ref="AP7:AP8"/>
-    <mergeCell ref="AQ7:AQ8"/>
-    <mergeCell ref="AR7:AR8"/>
-    <mergeCell ref="AL7:AL8"/>
-    <mergeCell ref="AN7:AN8"/>
-    <mergeCell ref="AO7:AO8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AK7:AK8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-330: Gesuchsteller Excel Tabellen angepasst und Code ergänzt
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wian\repos\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF8476B-EE38-4531-A2F3-8530A9BA1311}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2AB249-886B-4F03-B90E-7BD6166E172D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="720" windowWidth="16380" windowHeight="8190" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
   <si>
     <t>Parameter</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Diplomat</t>
   </si>
   <si>
-    <t>Erwerbspensum</t>
-  </si>
-  <si>
     <t>Situation</t>
   </si>
   <si>
@@ -119,15 +116,9 @@
     <t>Angestellt</t>
   </si>
   <si>
-    <t>Ausbildung</t>
-  </si>
-  <si>
     <t>Selbständig</t>
   </si>
   <si>
-    <t>RAV</t>
-  </si>
-  <si>
     <t>{institution}</t>
   </si>
   <si>
@@ -188,9 +179,6 @@
     <t>{gs1EwpGesundhtl}</t>
   </si>
   <si>
-    <t>Gesundheitliche Einschränkung</t>
-  </si>
-  <si>
     <t>{gs2Name}</t>
   </si>
   <si>
@@ -279,6 +267,27 @@
   </si>
   <si>
     <t>Gesuchsteller</t>
+  </si>
+  <si>
+    <t>In Aus- oder Weiterbildung</t>
+  </si>
+  <si>
+    <t>Arbeitssuchend</t>
+  </si>
+  <si>
+    <t>Gesundheitliche Indikation</t>
+  </si>
+  <si>
+    <t>In Integrations- oder Beschäftigungsprogramm</t>
+  </si>
+  <si>
+    <t>Beschäftigungspensum</t>
+  </si>
+  <si>
+    <t>{gs1EwpIntegration}</t>
+  </si>
+  <si>
+    <t>{gs2EwpIntegration}</t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -472,41 +481,44 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,10 +929,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AU9"/>
+  <dimension ref="A1:AW9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN13" sqref="AN13"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK12" sqref="AK12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,26 +941,34 @@
     <col min="3" max="3" width="15.7109375" style="1"/>
     <col min="4" max="5" width="17"/>
     <col min="7" max="15" width="8.7109375"/>
-    <col min="16" max="20" width="10.7109375"/>
-    <col min="21" max="21" width="24.140625"/>
-    <col min="22" max="30" width="8.7109375"/>
-    <col min="31" max="35" width="10.7109375"/>
-    <col min="36" max="36" width="24.140625"/>
-    <col min="37" max="37" width="9.140625" customWidth="1"/>
-    <col min="38" max="38" width="6.5703125"/>
-    <col min="39" max="39" width="18.140625"/>
-    <col min="41" max="41" width="23.28515625"/>
-    <col min="42" max="42" width="9.28515625"/>
-    <col min="43" max="43" width="25.42578125"/>
-    <col min="44" max="44" width="27.5703125"/>
-    <col min="45" max="45" width="10.5703125"/>
-    <col min="46" max="46" width="21.140625" customWidth="1"/>
-    <col min="47" max="1000" width="10.5703125"/>
+    <col min="16" max="17" width="10.7109375"/>
+    <col min="18" max="18" width="24.28515625" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375"/>
+    <col min="20" max="20" width="14.5703125" customWidth="1"/>
+    <col min="21" max="21" width="41.5703125" customWidth="1"/>
+    <col min="22" max="22" width="24.7109375" customWidth="1"/>
+    <col min="23" max="31" width="8.7109375"/>
+    <col min="32" max="33" width="10.7109375"/>
+    <col min="34" max="34" width="24.7109375" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375"/>
+    <col min="36" max="36" width="14.5703125" customWidth="1"/>
+    <col min="37" max="37" width="39.5703125" customWidth="1"/>
+    <col min="38" max="38" width="24.140625"/>
+    <col min="39" max="39" width="9.140625" customWidth="1"/>
+    <col min="40" max="40" width="6.5703125"/>
+    <col min="41" max="41" width="18.140625"/>
+    <col min="43" max="43" width="23.28515625"/>
+    <col min="44" max="44" width="9.28515625"/>
+    <col min="45" max="45" width="25.42578125"/>
+    <col min="46" max="46" width="27.5703125"/>
+    <col min="47" max="47" width="10.5703125"/>
+    <col min="48" max="48" width="21.140625" customWidth="1"/>
+    <col min="49" max="1002" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:49" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -956,10 +976,10 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -969,412 +989,441 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="6" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="21" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
-      <c r="AE6" s="30"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
-      <c r="AH6" s="30"/>
-      <c r="AI6" s="30"/>
-      <c r="AJ6" s="30"/>
-      <c r="AK6" s="23" t="s">
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="25"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="25"/>
+      <c r="AJ6" s="25"/>
+      <c r="AK6" s="25"/>
+      <c r="AL6" s="25"/>
+      <c r="AM6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="23" t="s">
+      <c r="AN6" s="26"/>
+      <c r="AO6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AN6" s="23"/>
-      <c r="AO6" s="23"/>
-      <c r="AP6" s="23"/>
-      <c r="AQ6" s="23"/>
-      <c r="AR6" s="23" t="s">
+      <c r="AP6" s="26"/>
+      <c r="AQ6" s="26"/>
+      <c r="AR6" s="26"/>
+      <c r="AS6" s="26"/>
+      <c r="AT6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="AS6" s="21" t="s">
+      <c r="AU6" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="21" t="s">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z7" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB7" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC7" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF7" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG7" s="28"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="28"/>
+      <c r="AJ7" s="28"/>
+      <c r="AK7" s="21"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="W7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="X7" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y7" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA7" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD7" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE7" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF7" s="25"/>
-      <c r="AG7" s="25"/>
-      <c r="AH7" s="25"/>
-      <c r="AI7" s="25"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="22" t="s">
+      <c r="AN7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="AL7" s="23" t="s">
+      <c r="AO7" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP7" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="AM7" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN7" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO7" s="23" t="s">
+      <c r="AR7" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS7" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AP7" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="AR7" s="23"/>
-      <c r="AS7" s="21"/>
+      <c r="AT7" s="26"/>
+      <c r="AU7" s="24"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
       <c r="P8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="Q8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="S8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="T8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="U8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="V8" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH8" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM8" s="26"/>
+      <c r="AN8" s="26"/>
+      <c r="AO8" s="32"/>
+      <c r="AP8" s="32"/>
+      <c r="AQ8" s="26"/>
+      <c r="AR8" s="26"/>
+      <c r="AS8" s="26"/>
+      <c r="AT8" s="26"/>
+      <c r="AU8" s="24"/>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="U8" s="13" t="s">
+      <c r="D9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="18" t="e">
+        <f>Q9+R9+S9+T9+V9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="U9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="V9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="W9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="X9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
-      <c r="AE8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ8" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK8" s="23"/>
-      <c r="AL8" s="23"/>
-      <c r="AM8" s="28"/>
-      <c r="AN8" s="28"/>
-      <c r="AO8" s="23"/>
-      <c r="AP8" s="23"/>
-      <c r="AQ8" s="23"/>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="21"/>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" s="18" t="e">
-        <f>Q9+R9+S9+T9+U9</f>
+      <c r="AA9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF9" s="19" t="e">
+        <f>IF((AG9+AH9+AI9+AJ9+AL9)&gt;0,AG9+AH9+AI9+AJ9+AL9,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="T9" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="U9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="V9" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="W9" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="X9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA9" s="11" t="s">
+      <c r="AG9" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="AB9" s="11" t="s">
+      <c r="AH9" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="AC9" s="11" t="s">
+      <c r="AI9" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="AD9" s="11" t="s">
+      <c r="AJ9" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="AE9" s="19" t="e">
-        <f>IF((AF9+AG9+AH9+AI9+AJ9)&gt;0,AF9+AG9+AH9+AI9+AJ9,)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AF9" s="16" t="s">
+      <c r="AK9" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL9" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="AG9" s="16" t="s">
+      <c r="AM9" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AH9" s="16" t="s">
+      <c r="AN9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AI9" s="16" t="s">
+      <c r="AO9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP9" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ9" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AJ9" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK9" s="11" t="s">
+      <c r="AS9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="AL9" s="11" t="s">
+      <c r="AT9" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="AM9" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN9" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO9" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP9" s="11" t="s">
+      <c r="AU9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="AQ9" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR9" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AS9" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT9" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="AU9" s="8"/>
+      <c r="AV9" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW9" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="AO6:AS6"/>
+    <mergeCell ref="AT6:AT8"/>
+    <mergeCell ref="AU6:AU8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AE8"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AN7:AN8"/>
+    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="AR7:AR8"/>
+    <mergeCell ref="AS7:AS8"/>
+    <mergeCell ref="AO7:AO8"/>
+    <mergeCell ref="AP7:AP8"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:U6"/>
-    <mergeCell ref="V6:AJ6"/>
-    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="G6:V6"/>
+    <mergeCell ref="W6:AL6"/>
+    <mergeCell ref="AM6:AN6"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
@@ -1385,26 +1434,13 @@
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="P7:T7"/>
-    <mergeCell ref="V7:V8"/>
     <mergeCell ref="W7:W8"/>
-    <mergeCell ref="AM6:AQ6"/>
-    <mergeCell ref="AR6:AR8"/>
-    <mergeCell ref="AS6:AS8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AI7"/>
-    <mergeCell ref="AL7:AL8"/>
-    <mergeCell ref="AO7:AO8"/>
-    <mergeCell ref="AP7:AP8"/>
-    <mergeCell ref="AQ7:AQ8"/>
-    <mergeCell ref="AM7:AM8"/>
-    <mergeCell ref="AN7:AN8"/>
     <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AK7:AK8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-330: Formel im Excel korrigiert
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wian\repos\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2AB249-886B-4F03-B90E-7BD6166E172D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8384F1BB-6A47-4881-9EF6-B2C3A71D6291}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="720" windowWidth="16380" windowHeight="8190" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -931,8 +932,8 @@
   </sheetPr>
   <dimension ref="A1:AW9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK12" sqref="AK12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1299,7 @@
         <v>43</v>
       </c>
       <c r="P9" s="18" t="e">
-        <f>Q9+R9+S9+T9+V9</f>
+        <f>Q9+R9+S9+T9+U9+V9</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q9" s="16" t="s">
@@ -1347,7 +1348,7 @@
         <v>57</v>
       </c>
       <c r="AF9" s="19" t="e">
-        <f>IF((AG9+AH9+AI9+AJ9+AL9)&gt;0,AG9+AH9+AI9+AJ9+AL9,)</f>
+        <f>IF((AG9+AH9+AI9+AJ9+AK+AL9)&gt;0,AG9+AH9+AI9+AJ9+AK+AL9,)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AG9" s="16" t="s">

</xml_diff>

<commit_message>
KIBON-120: Gesuchsteller statistic translated - All unused methods removed from ReportResource. They aren't used because we only execute them asynchronously which is implemented in ReportResourceAsync
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33590E7C-B817-44B5-AC23-5675934A7B64}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DBD2FC-9272-4CDA-9C92-540E1462863E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="720" windowWidth="16380" windowHeight="8190" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,93 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
   <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Angebot</t>
-  </si>
-  <si>
-    <t>Periode</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Eingangsdatum</t>
-  </si>
-  <si>
-    <t>Verfügungsdatum</t>
-  </si>
-  <si>
-    <t>Gesuchsteller 1</t>
-  </si>
-  <si>
-    <t>Gesuchsteller 2</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Fall-ID</t>
-  </si>
-  <si>
-    <t>Familie</t>
-  </si>
-  <si>
-    <t>Einkommen</t>
-  </si>
-  <si>
-    <t>Geprüft durch Steuerverwaltung</t>
-  </si>
-  <si>
-    <t>Veranlagt</t>
-  </si>
-  <si>
-    <t>Strasse</t>
-  </si>
-  <si>
-    <t>Nr</t>
-  </si>
-  <si>
-    <t>Zusatz</t>
-  </si>
-  <si>
-    <t>Plz</t>
-  </si>
-  <si>
-    <t>Ort</t>
-  </si>
-  <si>
-    <t>EWK-ID</t>
-  </si>
-  <si>
-    <t>Diplomat</t>
-  </si>
-  <si>
-    <t>Situation</t>
-  </si>
-  <si>
-    <t>Grösse</t>
-  </si>
-  <si>
-    <t>Massgebendes Einkommen</t>
-  </si>
-  <si>
-    <t>Einkommensverschlechterung</t>
-  </si>
-  <si>
-    <t>Angestellt</t>
-  </si>
-  <si>
-    <t>Selbständig</t>
-  </si>
-  <si>
     <t>{institution}</t>
   </si>
   <si>
@@ -231,9 +144,6 @@
     <t>{einkommensjahr}</t>
   </si>
   <si>
-    <t>Einkommensjahr</t>
-  </si>
-  <si>
     <t>{ekvVorhanden}</t>
   </si>
   <si>
@@ -246,49 +156,139 @@
     <t>{repeatRow}</t>
   </si>
   <si>
-    <t>Anrechenbares Einkommen vor Familienabzug</t>
-  </si>
-  <si>
     <t>{massgEinkVorFamilienabzug}</t>
   </si>
   <si>
-    <t>Familienabzug</t>
-  </si>
-  <si>
     <t>{familienabzug}</t>
   </si>
   <si>
     <t>{massgEink}</t>
   </si>
   <si>
-    <t>Stichtag</t>
-  </si>
-  <si>
     <t>{stichtag}</t>
   </si>
   <si>
-    <t>Gesuchsteller</t>
-  </si>
-  <si>
-    <t>In Aus- oder Weiterbildung</t>
-  </si>
-  <si>
-    <t>Arbeitssuchend</t>
-  </si>
-  <si>
-    <t>Gesundheitliche Indikation</t>
-  </si>
-  <si>
-    <t>In Integrations- oder Beschäftigungsprogramm</t>
-  </si>
-  <si>
-    <t>Beschäftigungspensum</t>
-  </si>
-  <si>
     <t>{gs1EwpIntegration}</t>
   </si>
   <si>
     <t>{gs2EwpIntegration}</t>
+  </si>
+  <si>
+    <t>{gesuchstellerTitle}</t>
+  </si>
+  <si>
+    <t>{stichtagTitle}</t>
+  </si>
+  <si>
+    <t>{institutionTitle}</t>
+  </si>
+  <si>
+    <t>{angebotTitle}</t>
+  </si>
+  <si>
+    <t>{parameterTitle}</t>
+  </si>
+  <si>
+    <t>{periodeTitle}</t>
+  </si>
+  <si>
+    <t>{eingangsdatumTitle}</t>
+  </si>
+  <si>
+    <t>{verfuegungsdatumTitle}</t>
+  </si>
+  <si>
+    <t>{fallIdTitle}</t>
+  </si>
+  <si>
+    <t>{gesuchsteller1Title}</t>
+  </si>
+  <si>
+    <t>{nachnameTitle}</t>
+  </si>
+  <si>
+    <t>{vornameTitle}</t>
+  </si>
+  <si>
+    <t>{strasseTitle}</t>
+  </si>
+  <si>
+    <t>{strasseNrTitel}</t>
+  </si>
+  <si>
+    <t>{zusatzTitle}</t>
+  </si>
+  <si>
+    <t>{plzTitle}</t>
+  </si>
+  <si>
+    <t>{ortTitle}</t>
+  </si>
+  <si>
+    <t>{ewkTitle}</t>
+  </si>
+  <si>
+    <t>{diplomatTitle}</t>
+  </si>
+  <si>
+    <t>{beschaeftigungspensumTitle}</t>
+  </si>
+  <si>
+    <t>{totalTitle}</t>
+  </si>
+  <si>
+    <t>{angestelltTitle}</t>
+  </si>
+  <si>
+    <t>{weiterbildungTitle}</t>
+  </si>
+  <si>
+    <t>{selbstaendigTitle}</t>
+  </si>
+  <si>
+    <t>{arbeitssuchendTitle}</t>
+  </si>
+  <si>
+    <t>{gesIndikationTitle}</t>
+  </si>
+  <si>
+    <t>{gesuchsteller2Title}</t>
+  </si>
+  <si>
+    <t>{familieTitle}</t>
+  </si>
+  <si>
+    <t>{famSituationTitle}</t>
+  </si>
+  <si>
+    <t>{famGroesseTitle}</t>
+  </si>
+  <si>
+    <t>{einkommenTitle}</t>
+  </si>
+  <si>
+    <t>{einkommenVorAbzugTitle}</t>
+  </si>
+  <si>
+    <t>{famAbzugTitle}</t>
+  </si>
+  <si>
+    <t>{massEinkommenTitle}</t>
+  </si>
+  <si>
+    <t>{einkommensjahrTitle}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungTitle}</t>
+  </si>
+  <si>
+    <t>{geprueftSTVTitle}</t>
+  </si>
+  <si>
+    <t>{veranlagtTitle}</t>
+  </si>
+  <si>
+    <t>{integrationTitle}</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -472,9 +472,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -486,40 +483,37 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,8 +926,8 @@
   </sheetPr>
   <dimension ref="A1:AW9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF10" sqref="AF10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +963,7 @@
   <sheetData>
     <row r="1" spans="1:49" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -982,7 +976,7 @@
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -992,422 +986,435 @@
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C4"/>
     </row>
     <row r="6" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="31"/>
-      <c r="AG6" s="31"/>
-      <c r="AH6" s="31"/>
-      <c r="AI6" s="31"/>
-      <c r="AJ6" s="31"/>
-      <c r="AK6" s="31"/>
-      <c r="AL6" s="31"/>
-      <c r="AM6" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN6" s="24"/>
-      <c r="AO6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AP6" s="24"/>
-      <c r="AQ6" s="24"/>
-      <c r="AR6" s="24"/>
-      <c r="AS6" s="24"/>
-      <c r="AT6" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="AU6" s="22" t="s">
-        <v>15</v>
+      <c r="A6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="24"/>
+      <c r="AI6" s="24"/>
+      <c r="AJ6" s="24"/>
+      <c r="AK6" s="24"/>
+      <c r="AL6" s="24"/>
+      <c r="AM6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN6" s="25"/>
+      <c r="AO6" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP6" s="25"/>
+      <c r="AQ6" s="25"/>
+      <c r="AR6" s="25"/>
+      <c r="AS6" s="25"/>
+      <c r="AT6" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU6" s="23" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="21"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="20"/>
       <c r="V7" s="9"/>
-      <c r="W7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="X7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y7" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA7" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB7" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD7" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF7" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG7" s="26"/>
-      <c r="AH7" s="26"/>
-      <c r="AI7" s="26"/>
-      <c r="AJ7" s="26"/>
-      <c r="AK7" s="21"/>
+      <c r="W7" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="X7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y7" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z7" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB7" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC7" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD7" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE7" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF7" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="27"/>
+      <c r="AI7" s="27"/>
+      <c r="AJ7" s="27"/>
+      <c r="AK7" s="20"/>
       <c r="AL7" s="9"/>
-      <c r="AM7" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="AN7" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="AO7" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP7" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ7" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="AR7" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS7" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="AT7" s="24"/>
-      <c r="AU7" s="22"/>
+      <c r="AM7" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN7" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO7" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP7" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ7" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR7" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS7" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="AT7" s="25"/>
+      <c r="AU7" s="23"/>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
       <c r="P8" s="12" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="V8" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="22"/>
+        <v>72</v>
+      </c>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23"/>
+      <c r="AE8" s="23"/>
       <c r="AF8" s="12" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="AH8" s="12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="AI8" s="12" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="AJ8" s="12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL8" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM8" s="24"/>
-      <c r="AN8" s="24"/>
-      <c r="AO8" s="29"/>
-      <c r="AP8" s="29"/>
-      <c r="AQ8" s="24"/>
-      <c r="AR8" s="24"/>
-      <c r="AS8" s="24"/>
-      <c r="AT8" s="24"/>
-      <c r="AU8" s="22"/>
+        <v>85</v>
+      </c>
+      <c r="AL8" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM8" s="25"/>
+      <c r="AN8" s="25"/>
+      <c r="AO8" s="30"/>
+      <c r="AP8" s="30"/>
+      <c r="AQ8" s="25"/>
+      <c r="AR8" s="25"/>
+      <c r="AS8" s="25"/>
+      <c r="AT8" s="25"/>
+      <c r="AU8" s="23"/>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>4</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9" s="18" t="e">
+        <v>14</v>
+      </c>
+      <c r="P9" s="17" t="e">
         <f>Q9+R9+S9+T9+U9+V9</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="R9" s="16" t="s">
+      <c r="Q9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="S9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="T9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="S9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="U9" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="V9" s="16" t="s">
-        <v>48</v>
+      <c r="V9" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="W9" s="11" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="X9" s="11" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="Y9" s="11" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="AB9" s="11" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="AD9" s="11" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="AE9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF9" s="19" t="e">
+        <v>28</v>
+      </c>
+      <c r="AF9" s="18" t="e">
         <f>IF((AG9+AH9+AI9+AJ9+AK9+AL9)&gt;0,AG9+AH9+AI9+AJ9+AK9+AL9,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AG9" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH9" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI9" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ9" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK9" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL9" s="16" t="s">
-        <v>62</v>
+      <c r="AG9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL9" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="AM9" s="11" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="AN9" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO9" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP9" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="AQ9" s="17" t="s">
-        <v>75</v>
+        <v>35</v>
+      </c>
+      <c r="AO9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ9" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="AR9" s="11" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="AS9" s="11" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="AT9" s="11" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="AU9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV9" s="20" t="s">
-        <v>70</v>
+        <v>39</v>
+      </c>
+      <c r="AV9" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AW9" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="AO6:AS6"/>
+    <mergeCell ref="AT6:AT8"/>
+    <mergeCell ref="AU6:AU8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AE8"/>
+    <mergeCell ref="AF7:AJ7"/>
+    <mergeCell ref="AN7:AN8"/>
+    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="AR7:AR8"/>
+    <mergeCell ref="AS7:AS8"/>
+    <mergeCell ref="AO7:AO8"/>
+    <mergeCell ref="AP7:AP8"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="G6:V6"/>
     <mergeCell ref="W6:AL6"/>
@@ -1424,24 +1431,11 @@
     <mergeCell ref="P7:T7"/>
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
-    <mergeCell ref="AO6:AS6"/>
-    <mergeCell ref="AT6:AT8"/>
-    <mergeCell ref="AU6:AU8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AE8"/>
-    <mergeCell ref="AF7:AJ7"/>
-    <mergeCell ref="AN7:AN8"/>
-    <mergeCell ref="AQ7:AQ8"/>
-    <mergeCell ref="AR7:AR8"/>
-    <mergeCell ref="AS7:AS8"/>
-    <mergeCell ref="AO7:AO8"/>
-    <mergeCell ref="AP7:AP8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2118: split ekv into ekv1/ekv2 and annulliert fields in excel template
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572B1FD4-2A88-4EAE-9A72-D4018A3F7614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F0103-B208-45EB-9506-E47B0D2E8621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
   <si>
     <t>{institution}</t>
   </si>
@@ -140,9 +140,6 @@
     <t>{einkommensjahr}</t>
   </si>
   <si>
-    <t>{ekvVorhanden}</t>
-  </si>
-  <si>
     <t>{stvGeprueft}</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>{einkommensjahrTitle}</t>
   </si>
   <si>
-    <t>{einkommensverschlechterungTitle}</t>
-  </si>
-  <si>
     <t>{geprueftSTVTitle}</t>
   </si>
   <si>
@@ -288,6 +282,30 @@
   </si>
   <si>
     <t>{gemeinde}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungBasisJahr1Title}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungBasisJahr2Title}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungBasisJahr1AnnuliertTitle}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungBasisJahr2AnnuliertTitle}</t>
+  </si>
+  <si>
+    <t>{ekvVorhandenBasisJahr1}</t>
+  </si>
+  <si>
+    <t>{ekvVorhandenBasisJahr2}</t>
+  </si>
+  <si>
+    <t>{ekvAnnuliertBasisJahr1}</t>
+  </si>
+  <si>
+    <t>{ekvAnnuliertBasisJahr2}</t>
   </si>
 </sst>
 </file>
@@ -441,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -482,36 +500,42 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -923,9 +947,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AV9"/>
+  <dimension ref="A1:AY9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR17" sqref="AR17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -952,15 +978,15 @@
     <col min="42" max="42" width="23.28515625"/>
     <col min="43" max="43" width="9.28515625"/>
     <col min="44" max="44" width="25.42578125"/>
-    <col min="45" max="45" width="27.5703125"/>
-    <col min="46" max="46" width="10.5703125"/>
-    <col min="47" max="47" width="21.140625" customWidth="1"/>
-    <col min="48" max="1001" width="10.5703125"/>
+    <col min="48" max="48" width="27.5703125"/>
+    <col min="49" max="49" width="10.5703125"/>
+    <col min="50" max="50" width="21.140625" customWidth="1"/>
+    <col min="51" max="1004" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -969,12 +995,12 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -983,264 +1009,279 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="6" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="F6" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="21" t="s">
+      <c r="H6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="21"/>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="30"/>
+      <c r="AG6" s="30"/>
+      <c r="AH6" s="30"/>
+      <c r="AI6" s="30"/>
+      <c r="AJ6" s="30"/>
+      <c r="AK6" s="30"/>
+      <c r="AL6" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO6" s="33"/>
+      <c r="AP6" s="33"/>
+      <c r="AQ6" s="33"/>
+      <c r="AR6" s="33"/>
+      <c r="AS6" s="33"/>
+      <c r="AT6" s="33"/>
+      <c r="AU6" s="22"/>
+      <c r="AV6" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW6" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
-      <c r="AI6" s="24"/>
-      <c r="AJ6" s="24"/>
-      <c r="AK6" s="24"/>
-      <c r="AL6" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM6" s="25"/>
-      <c r="AN6" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO6" s="25"/>
-      <c r="AP6" s="25"/>
-      <c r="AQ6" s="25"/>
-      <c r="AR6" s="25"/>
-      <c r="AS6" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="AT6" s="23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="23" t="s">
+      <c r="I7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="J7" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="K7" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="L7" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="M7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="N7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="23" t="s">
+      <c r="O7" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="P7" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="P7" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
       <c r="U7" s="20"/>
       <c r="V7" s="9"/>
-      <c r="W7" s="23" t="s">
+      <c r="W7" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="X7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="X7" s="23" t="s">
+      <c r="Y7" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="Y7" s="23" t="s">
+      <c r="Z7" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="Z7" s="23" t="s">
+      <c r="AA7" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AA7" s="23" t="s">
+      <c r="AB7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AB7" s="23" t="s">
+      <c r="AC7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AC7" s="23" t="s">
+      <c r="AD7" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="AD7" s="26" t="s">
+      <c r="AE7" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="AE7" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
-      <c r="AH7" s="27"/>
-      <c r="AI7" s="27"/>
+      <c r="AF7" s="25"/>
+      <c r="AG7" s="25"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="25"/>
       <c r="AJ7" s="20"/>
       <c r="AK7" s="9"/>
-      <c r="AL7" s="31" t="s">
+      <c r="AL7" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM7" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="AM7" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN7" s="29" t="s">
+      <c r="AN7" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO7" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="AO7" s="29" t="s">
+      <c r="AP7" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="AP7" s="25" t="s">
+      <c r="AQ7" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="AQ7" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="AR7" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="AS7" s="25"/>
-      <c r="AT7" s="23"/>
+      <c r="AR7" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS7" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT7" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU7" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV7" s="23"/>
+      <c r="AW7" s="21"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
       <c r="P8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q8" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="R8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="S8" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="T8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="U8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="V8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U8" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="V8" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
       <c r="AE8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF8" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="AF8" s="12" t="s">
+      <c r="AG8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="AG8" s="12" t="s">
+      <c r="AH8" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AH8" s="12" t="s">
+      <c r="AI8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AI8" s="12" t="s">
+      <c r="AJ8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AJ8" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK8" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL8" s="25"/>
-      <c r="AM8" s="25"/>
-      <c r="AN8" s="30"/>
-      <c r="AO8" s="30"/>
-      <c r="AP8" s="25"/>
-      <c r="AQ8" s="25"/>
-      <c r="AR8" s="25"/>
-      <c r="AS8" s="25"/>
-      <c r="AT8" s="23"/>
+      <c r="AL8" s="23"/>
+      <c r="AM8" s="23"/>
+      <c r="AN8" s="28"/>
+      <c r="AO8" s="28"/>
+      <c r="AP8" s="23"/>
+      <c r="AQ8" s="23"/>
+      <c r="AR8" s="26"/>
+      <c r="AS8" s="28"/>
+      <c r="AT8" s="28"/>
+      <c r="AU8" s="28"/>
+      <c r="AV8" s="23"/>
+      <c r="AW8" s="21"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1298,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>5</v>
@@ -1303,7 +1344,7 @@
         <v>17</v>
       </c>
       <c r="U9" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V9" s="15" t="s">
         <v>18</v>
@@ -1349,7 +1390,7 @@
         <v>30</v>
       </c>
       <c r="AJ9" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK9" s="15" t="s">
         <v>31</v>
@@ -1361,49 +1402,48 @@
         <v>33</v>
       </c>
       <c r="AN9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AO9" s="16" t="s">
+      <c r="AP9" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="AP9" s="16" t="s">
-        <v>41</v>
       </c>
       <c r="AQ9" s="11" t="s">
         <v>34</v>
       </c>
       <c r="AR9" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS9" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="AT9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU9" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="11" t="s">
+      <c r="AW9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AT9" s="11" t="s">
+      <c r="AX9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AU9" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV9" s="8"/>
+      <c r="AY9" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AL7:AL8"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS6:AS8"/>
-    <mergeCell ref="AT6:AT8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AI7"/>
-    <mergeCell ref="AM7:AM8"/>
-    <mergeCell ref="AP7:AP8"/>
-    <mergeCell ref="AQ7:AQ8"/>
-    <mergeCell ref="AR7:AR8"/>
-    <mergeCell ref="AN7:AN8"/>
-    <mergeCell ref="AO7:AO8"/>
+  <mergeCells count="41">
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="H6:V6"/>
     <mergeCell ref="W6:AK6"/>
@@ -1420,12 +1460,25 @@
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
     <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="AV6:AV8"/>
+    <mergeCell ref="AW6:AW8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AI7"/>
+    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="AP7:AP8"/>
+    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="AR7:AR8"/>
+    <mergeCell ref="AN7:AN8"/>
+    <mergeCell ref="AO7:AO8"/>
+    <mergeCell ref="AS7:AS8"/>
+    <mergeCell ref="AT7:AT8"/>
+    <mergeCell ref="AU7:AU8"/>
+    <mergeCell ref="AN6:AU6"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AL7:AL8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2166: add mzvBeantragt to Antragstellende statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F0103-B208-45EB-9506-E47B0D2E8621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511CC420-2F8F-463B-979B-547E5DDE139F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>{institution}</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>{ekvAnnuliertBasisJahr2}</t>
+  </si>
+  <si>
+    <t>{mzvBeantragtTitle}</t>
+  </si>
+  <si>
+    <t>{mzvBeantragt}</t>
   </si>
 </sst>
 </file>
@@ -523,6 +529,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -531,12 +543,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,10 +953,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AY9"/>
+  <dimension ref="A1:AZ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR17" sqref="AR17"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AW6" sqref="AW6:AW8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,12 +985,13 @@
     <col min="43" max="43" width="9.28515625"/>
     <col min="44" max="44" width="25.42578125"/>
     <col min="48" max="48" width="27.5703125"/>
-    <col min="49" max="49" width="10.5703125"/>
-    <col min="50" max="50" width="21.140625" customWidth="1"/>
-    <col min="51" max="1004" width="10.5703125"/>
+    <col min="49" max="49" width="12.42578125" customWidth="1"/>
+    <col min="50" max="50" width="10.5703125"/>
+    <col min="51" max="51" width="21.140625" customWidth="1"/>
+    <col min="52" max="1005" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:52" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -995,10 +1002,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
@@ -1009,7 +1016,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1018,26 +1025,26 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="6" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="31" t="s">
         <v>52</v>
       </c>
       <c r="H6" s="21" t="s">
@@ -1050,13 +1057,13 @@
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
       <c r="W6" s="21" t="s">
         <v>69</v>
       </c>
@@ -1067,42 +1074,45 @@
       <c r="AB6" s="21"/>
       <c r="AC6" s="21"/>
       <c r="AD6" s="21"/>
-      <c r="AE6" s="30"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
-      <c r="AH6" s="30"/>
-      <c r="AI6" s="30"/>
-      <c r="AJ6" s="30"/>
-      <c r="AK6" s="30"/>
+      <c r="AE6" s="32"/>
+      <c r="AF6" s="32"/>
+      <c r="AG6" s="32"/>
+      <c r="AH6" s="32"/>
+      <c r="AI6" s="32"/>
+      <c r="AJ6" s="32"/>
+      <c r="AK6" s="32"/>
       <c r="AL6" s="23" t="s">
         <v>70</v>
       </c>
       <c r="AM6" s="23"/>
-      <c r="AN6" s="32" t="s">
+      <c r="AN6" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="AO6" s="33"/>
-      <c r="AP6" s="33"/>
-      <c r="AQ6" s="33"/>
-      <c r="AR6" s="33"/>
-      <c r="AS6" s="33"/>
-      <c r="AT6" s="33"/>
+      <c r="AO6" s="30"/>
+      <c r="AP6" s="30"/>
+      <c r="AQ6" s="30"/>
+      <c r="AR6" s="30"/>
+      <c r="AS6" s="30"/>
+      <c r="AT6" s="30"/>
       <c r="AU6" s="22"/>
       <c r="AV6" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="AW6" s="21" t="s">
+      <c r="AW6" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX6" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+    <row r="7" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
       <c r="H7" s="21" t="s">
         <v>54</v>
       </c>
@@ -1200,16 +1210,17 @@
         <v>86</v>
       </c>
       <c r="AV7" s="23"/>
-      <c r="AW7" s="21"/>
+      <c r="AW7" s="23"/>
+      <c r="AX7" s="21"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
@@ -1279,9 +1290,10 @@
       <c r="AT8" s="28"/>
       <c r="AU8" s="28"/>
       <c r="AV8" s="23"/>
-      <c r="AW8" s="21"/>
+      <c r="AW8" s="23"/>
+      <c r="AX8" s="21"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>0</v>
       </c>
@@ -1429,15 +1441,18 @@
         <v>35</v>
       </c>
       <c r="AW9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="AX9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="19" t="s">
+      <c r="AY9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AY9" s="8"/>
+      <c r="AZ9" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="42">
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
@@ -1460,8 +1475,7 @@
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="X7:X8"/>
     <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="AV6:AV8"/>
-    <mergeCell ref="AW6:AW8"/>
+    <mergeCell ref="AX6:AX8"/>
     <mergeCell ref="AC7:AC8"/>
     <mergeCell ref="AD7:AD8"/>
     <mergeCell ref="AE7:AI7"/>
@@ -1479,6 +1493,8 @@
     <mergeCell ref="AA7:AA8"/>
     <mergeCell ref="AB7:AB8"/>
     <mergeCell ref="AL7:AL8"/>
+    <mergeCell ref="AW6:AW8"/>
+    <mergeCell ref="AV6:AV8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>